<commit_message>
All variables collected from Timetables
</commit_message>
<xml_diff>
--- a/csv/Timetables rated.xlsx
+++ b/csv/Timetables rated.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bolup\OneDrive\Documents\Projizzles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a9b5661b6c851ed/Documents/Projizzles/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8568FC7B-05AB-47D3-9AEE-E44B3F9AFABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{8568FC7B-05AB-47D3-9AEE-E44B3F9AFABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B0D5B0A-1DFC-47CF-8785-F8DFA1C5DD1C}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="7320" yWindow="-60" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timetables rated" sheetId="1" r:id="rId1"/>
@@ -1525,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,12 +1536,12 @@
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="11" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="18.7109375" style="3" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
@@ -4237,7 +4237,7 @@
         <v>12</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="10">D34/B34</f>
+        <f t="shared" ref="E34:E61" si="10">D34/B34</f>
         <v>2.4</v>
       </c>
       <c r="F34" s="1">
@@ -4249,7 +4249,7 @@
         <v>2.4</v>
       </c>
       <c r="H34">
-        <f t="shared" ref="H34:H65" si="13">F34/G34</f>
+        <f t="shared" ref="H34:H61" si="13">F34/G34</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="I34">
@@ -4265,7 +4265,7 @@
         <v>3</v>
       </c>
       <c r="M34">
-        <f t="shared" ref="M34:M65" si="14">L34/5</f>
+        <f t="shared" ref="M34:M61" si="14">L34/5</f>
         <v>0.6</v>
       </c>
       <c r="N34">
@@ -4273,14 +4273,14 @@
         <v>1</v>
       </c>
       <c r="O34" s="1">
-        <f t="shared" ref="O34:O65" si="16">F34/N34</f>
+        <f t="shared" ref="O34:O61" si="16">F34/N34</f>
         <v>4</v>
       </c>
       <c r="P34" s="1">
         <v>4</v>
       </c>
       <c r="Q34">
-        <f t="shared" ref="Q34:Q65" si="17">((P34-(MIN(P:P)))^2)/((MAX(P:P)-MIN(P:P))^2)</f>
+        <f t="shared" ref="Q34:Q61" si="17">((P34-(MIN(P:P)))^2)/((MAX(P:P)-MIN(P:P))^2)</f>
         <v>0.25</v>
       </c>
       <c r="R34" s="1">
@@ -4299,7 +4299,7 @@
         <v>49</v>
       </c>
       <c r="X34">
-        <f t="shared" ref="X34:X65" si="18">IF(W34="Bad",0,IF(W34="Bad-N",0,IF(W34="Good-N",1,IF(W34="Good",1,"bruhm"))))</f>
+        <f t="shared" ref="X34:X61" si="18">IF(W34="Bad",0,IF(W34="Bad-N",0,IF(W34="Good-N",1,IF(W34="Good",1,"bruhm"))))</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>